<commit_message>
Testing done for original vs. rewritten
</commit_message>
<xml_diff>
--- a/sql_queries/Queries.xlsx
+++ b/sql_queries/Queries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suhas\Downloads\E0261_P11\sql_queries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E382FD-02D7-40C2-B62E-437763C01BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A29B49A-52BE-4A50-A3B0-00F03162B107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FD9CF7A0-92A1-4AFF-99B4-CDF3D003E942}"/>
   </bookViews>
@@ -17,12 +17,25 @@
     <sheet name="Original vs. Mutated" sheetId="2" r:id="rId2"/>
     <sheet name="Rewritten vs. Mutated" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="78">
   <si>
     <t>Query ID</t>
   </si>
@@ -217,6 +230,48 @@
   </si>
   <si>
     <t>UnionMergeRule</t>
+  </si>
+  <si>
+    <t>&lt;No transformations found&gt;</t>
+  </si>
+  <si>
+    <t>FilterJoinRule</t>
+  </si>
+  <si>
+    <t>AggregateUnionTransposeRule
+AggregateJoinTransposeRule
+SortRemoveRule</t>
+  </si>
+  <si>
+    <t>JoinConditionPushRule</t>
+  </si>
+  <si>
+    <t>JoinCommuteRule</t>
+  </si>
+  <si>
+    <t>ReduceExpressionsRule</t>
+  </si>
+  <si>
+    <t>ProjectRenameRule</t>
+  </si>
+  <si>
+    <t>ProjectTableScanRule</t>
+  </si>
+  <si>
+    <t>JoinAssociateRule
+JoinCommuteRule</t>
+  </si>
+  <si>
+    <t>FilterProjectTransposeRule</t>
+  </si>
+  <si>
+    <t>AggregateProjectMergeRule</t>
+  </si>
+  <si>
+    <t>True Positives</t>
+  </si>
+  <si>
+    <t>False Negatives</t>
   </si>
 </sst>
 </file>
@@ -700,9 +755,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1078,15 +1136,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F496A8C6-08C4-4A1F-98FE-4CD78283FFD1}">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.77734375" bestFit="1" customWidth="1"/>
@@ -1116,6 +1174,9 @@
       <c r="C2" t="s">
         <v>64</v>
       </c>
+      <c r="D2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -1127,6 +1188,9 @@
       <c r="C3" t="s">
         <v>64</v>
       </c>
+      <c r="D3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -1138,6 +1202,9 @@
       <c r="C4" t="s">
         <v>64</v>
       </c>
+      <c r="D4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -1149,6 +1216,9 @@
       <c r="C5" t="s">
         <v>64</v>
       </c>
+      <c r="D5" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -1160,6 +1230,9 @@
       <c r="C6" t="s">
         <v>64</v>
       </c>
+      <c r="D6" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -1171,6 +1244,9 @@
       <c r="C7" t="s">
         <v>64</v>
       </c>
+      <c r="D7" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -1182,48 +1258,120 @@
       <c r="C8" t="s">
         <v>64</v>
       </c>
+      <c r="D8" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B10" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="B14" t="b">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" t="b">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1233,220 +1381,600 @@
       <c r="C17" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B18" t="b">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B19" t="b">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B20" t="b">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B21" t="b">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B22" t="b">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B23" t="b">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B24" t="b">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B25" t="b">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B26" t="b">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B27" t="b">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B28" t="b">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B29" t="b">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B31" t="b">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B32" t="b">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B33" t="b">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B34" t="b">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B35" t="b">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B36" t="b">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B37" t="b">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B38" t="b">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B39" t="b">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B40" t="b">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>69</v>
+      </c>
+      <c r="D40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B41" t="b">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>65</v>
+      </c>
+      <c r="D41" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B42" t="b">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B43" t="b">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>70</v>
+      </c>
+      <c r="D43" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B44" t="b">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>71</v>
+      </c>
+      <c r="D44" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B45" t="b">
+        <v>1</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D45" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B46" t="b">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>72</v>
+      </c>
+      <c r="D46" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B47" t="b">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
+        <v>74</v>
+      </c>
+      <c r="D47" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B48" t="b">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>65</v>
+      </c>
+      <c r="D48" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B49" t="b">
+        <v>1</v>
+      </c>
+      <c r="C49" t="s">
+        <v>75</v>
+      </c>
+      <c r="D49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B50" t="b">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s">
+        <v>65</v>
+      </c>
+      <c r="D50" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B51" t="b">
+        <v>0</v>
+      </c>
+      <c r="C51" t="s">
+        <v>63</v>
+      </c>
+      <c r="D51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B52" t="b">
+        <v>1</v>
+      </c>
+      <c r="C52" t="s">
+        <v>72</v>
+      </c>
+      <c r="D52" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B53" t="b">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>65</v>
+      </c>
+      <c r="D53" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B54" t="b">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>65</v>
+      </c>
+      <c r="D54" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+      <c r="B55" t="b">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>71</v>
+      </c>
+      <c r="D55" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+      <c r="B56" t="b">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>70</v>
+      </c>
+      <c r="D56" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="B57" t="b">
+        <v>0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>63</v>
+      </c>
+      <c r="D57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+      <c r="B58" t="b">
+        <v>0</v>
+      </c>
+      <c r="C58" t="s">
+        <v>63</v>
+      </c>
+      <c r="D58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>59</v>
+        <v>76</v>
+      </c>
+      <c r="B60">
+        <f>COUNTIF(B2:B58,TRUE)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B61">
+        <f>COUNTIF(B2:B59,FALSE)</f>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1458,8 +1986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACAA0CA1-EA54-4853-8C38-9DEA75E9E66D}">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A2" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>